<commit_message>
Testing done on pulling from database! 3 small errors fixed! (Models.cpp)
</commit_message>
<xml_diff>
--- a/motherload_db_schema.xlsx
+++ b/motherload_db_schema.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="121">
   <si>
     <t>Inventory</t>
   </si>
@@ -371,13 +371,19 @@
     <t>…</t>
   </si>
   <si>
-    <t>InventoryItems</t>
+    <t>buildingX</t>
+  </si>
+  <si>
+    <t>buildingY</t>
+  </si>
+  <si>
+    <t>width</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -834,33 +840,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
@@ -878,23 +857,50 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="21" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="22" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="23" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1205,7 +1211,7 @@
   <dimension ref="B2:V45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K39" sqref="J39:K40"/>
+      <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1231,28 +1237,28 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:22" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="63" t="s">
         <v>57</v>
       </c>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="G2" s="37" t="s">
+      <c r="C2" s="63"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="63"/>
+      <c r="G2" s="63" t="s">
         <v>82</v>
       </c>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
-      <c r="K2" s="37"/>
-      <c r="L2" s="37"/>
-      <c r="M2" s="37"/>
-      <c r="R2" s="63" t="s">
+      <c r="H2" s="63"/>
+      <c r="I2" s="63"/>
+      <c r="J2" s="63"/>
+      <c r="K2" s="63"/>
+      <c r="L2" s="63"/>
+      <c r="M2" s="63"/>
+      <c r="R2" s="57" t="s">
         <v>114</v>
       </c>
-      <c r="S2" s="63"/>
-      <c r="T2" s="63"/>
-      <c r="U2" s="63"/>
-      <c r="V2" s="63"/>
+      <c r="S2" s="57"/>
+      <c r="T2" s="57"/>
+      <c r="U2" s="57"/>
+      <c r="V2" s="57"/>
     </row>
     <row r="3" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B3" s="23" t="s">
@@ -1288,19 +1294,19 @@
       <c r="M3" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="R3" s="51" t="s">
+      <c r="R3" s="42" t="s">
         <v>109</v>
       </c>
-      <c r="S3" s="48" t="s">
+      <c r="S3" s="39" t="s">
         <v>110</v>
       </c>
-      <c r="T3" s="48" t="s">
+      <c r="T3" s="39" t="s">
         <v>111</v>
       </c>
-      <c r="U3" s="48" t="s">
+      <c r="U3" s="39" t="s">
         <v>112</v>
       </c>
-      <c r="V3" s="50" t="s">
+      <c r="V3" s="41" t="s">
         <v>113</v>
       </c>
     </row>
@@ -1338,13 +1344,13 @@
       <c r="M4" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="R4" s="47" t="s">
+      <c r="R4" s="38" t="s">
         <v>57</v>
       </c>
-      <c r="S4" s="52"/>
-      <c r="T4" s="53"/>
-      <c r="U4" s="53"/>
-      <c r="V4" s="54"/>
+      <c r="S4" s="43"/>
+      <c r="T4" s="44"/>
+      <c r="U4" s="44"/>
+      <c r="V4" s="45"/>
     </row>
     <row r="5" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B5" s="3">
@@ -1380,13 +1386,13 @@
       <c r="M5" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="R5" s="47" t="s">
+      <c r="R5" s="38" t="s">
         <v>49</v>
       </c>
-      <c r="S5" s="55"/>
-      <c r="T5" s="56"/>
-      <c r="U5" s="56"/>
-      <c r="V5" s="57"/>
+      <c r="S5" s="46"/>
+      <c r="T5" s="47"/>
+      <c r="U5" s="47"/>
+      <c r="V5" s="48"/>
     </row>
     <row r="6" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B6" s="3">
@@ -1422,13 +1428,13 @@
       <c r="M6" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="R6" s="47" t="s">
+      <c r="R6" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="S6" s="55"/>
-      <c r="T6" s="56"/>
-      <c r="U6" s="56"/>
-      <c r="V6" s="57"/>
+      <c r="S6" s="46"/>
+      <c r="T6" s="47"/>
+      <c r="U6" s="47"/>
+      <c r="V6" s="48"/>
     </row>
     <row r="7" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B7" s="3">
@@ -1464,13 +1470,13 @@
       <c r="M7" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="R7" s="47" t="s">
+      <c r="R7" s="38" t="s">
         <v>66</v>
       </c>
-      <c r="S7" s="55"/>
-      <c r="T7" s="56"/>
-      <c r="U7" s="56"/>
-      <c r="V7" s="57"/>
+      <c r="S7" s="46"/>
+      <c r="T7" s="47"/>
+      <c r="U7" s="47"/>
+      <c r="V7" s="48"/>
     </row>
     <row r="8" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B8" s="3">
@@ -1506,13 +1512,13 @@
       <c r="M8" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="R8" s="47" t="s">
+      <c r="R8" s="38" t="s">
         <v>74</v>
       </c>
-      <c r="S8" s="55"/>
-      <c r="T8" s="56"/>
-      <c r="U8" s="56"/>
-      <c r="V8" s="57"/>
+      <c r="S8" s="46"/>
+      <c r="T8" s="47"/>
+      <c r="U8" s="47"/>
+      <c r="V8" s="48"/>
     </row>
     <row r="9" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="6">
@@ -1548,13 +1554,13 @@
       <c r="M9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="R9" s="47" t="s">
+      <c r="R9" s="38" t="s">
         <v>82</v>
       </c>
-      <c r="S9" s="55"/>
-      <c r="T9" s="56"/>
-      <c r="U9" s="56"/>
-      <c r="V9" s="57"/>
+      <c r="S9" s="46"/>
+      <c r="T9" s="47"/>
+      <c r="U9" s="47"/>
+      <c r="V9" s="48"/>
     </row>
     <row r="10" spans="2:22" x14ac:dyDescent="0.25">
       <c r="D10" s="11"/>
@@ -1580,21 +1586,21 @@
       <c r="M10" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="R10" s="47" t="s">
+      <c r="R10" s="38" t="s">
         <v>103</v>
       </c>
-      <c r="S10" s="55"/>
-      <c r="T10" s="56"/>
-      <c r="U10" s="56"/>
-      <c r="V10" s="57"/>
+      <c r="S10" s="46"/>
+      <c r="T10" s="47"/>
+      <c r="U10" s="47"/>
+      <c r="V10" s="48"/>
     </row>
     <row r="11" spans="2:22" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="37" t="s">
+      <c r="B11" s="63" t="s">
         <v>49</v>
       </c>
-      <c r="C11" s="37"/>
-      <c r="D11" s="37"/>
-      <c r="E11" s="37"/>
+      <c r="C11" s="63"/>
+      <c r="D11" s="63"/>
+      <c r="E11" s="63"/>
       <c r="G11" s="21">
         <v>7</v>
       </c>
@@ -1616,13 +1622,13 @@
       <c r="M11" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="R11" s="47" t="s">
-        <v>0</v>
-      </c>
-      <c r="S11" s="58"/>
-      <c r="T11" s="59"/>
-      <c r="U11" s="59"/>
-      <c r="V11" s="57"/>
+      <c r="R11" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="S11" s="49"/>
+      <c r="T11" s="50"/>
+      <c r="U11" s="50"/>
+      <c r="V11" s="48"/>
     </row>
     <row r="12" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B12" s="23" t="s">
@@ -1658,13 +1664,13 @@
       <c r="M12" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="R12" s="47" t="s">
+      <c r="R12" s="38" t="s">
         <v>101</v>
       </c>
-      <c r="S12" s="58"/>
-      <c r="T12" s="59"/>
-      <c r="U12" s="59"/>
-      <c r="V12" s="57"/>
+      <c r="S12" s="49"/>
+      <c r="T12" s="50"/>
+      <c r="U12" s="50"/>
+      <c r="V12" s="48"/>
     </row>
     <row r="13" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="3">
@@ -1700,13 +1706,13 @@
       <c r="M13" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="R13" s="49" t="s">
+      <c r="R13" s="40" t="s">
         <v>93</v>
       </c>
-      <c r="S13" s="60"/>
-      <c r="T13" s="61"/>
-      <c r="U13" s="61"/>
-      <c r="V13" s="62"/>
+      <c r="S13" s="51"/>
+      <c r="T13" s="52"/>
+      <c r="U13" s="52"/>
+      <c r="V13" s="53"/>
     </row>
     <row r="14" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="3">
@@ -1770,18 +1776,18 @@
       <c r="E16" s="16">
         <v>40</v>
       </c>
-      <c r="G16" s="37" t="s">
+      <c r="G16" s="63" t="s">
         <v>93</v>
       </c>
-      <c r="H16" s="37"/>
-      <c r="I16" s="37"/>
-      <c r="J16" s="37"/>
-      <c r="K16" s="37"/>
-      <c r="L16" s="37"/>
-      <c r="M16" s="37"/>
-      <c r="N16" s="37"/>
-      <c r="O16" s="37"/>
-      <c r="P16" s="37"/>
+      <c r="H16" s="63"/>
+      <c r="I16" s="63"/>
+      <c r="J16" s="63"/>
+      <c r="K16" s="63"/>
+      <c r="L16" s="63"/>
+      <c r="M16" s="63"/>
+      <c r="N16" s="63"/>
+      <c r="O16" s="63"/>
+      <c r="P16" s="63"/>
     </row>
     <row r="17" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
@@ -1808,21 +1814,21 @@
       <c r="J17" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="K17" s="42" t="s">
+      <c r="K17" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="L17" s="42"/>
+      <c r="L17" s="61"/>
       <c r="M17" s="24" t="s">
         <v>94</v>
       </c>
       <c r="N17" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="O17" s="68" t="s">
+      <c r="O17" s="67" t="s">
         <v>116</v>
       </c>
-      <c r="P17" s="68"/>
-      <c r="Q17" s="64" t="s">
+      <c r="P17" s="67"/>
+      <c r="Q17" s="54" t="s">
         <v>95</v>
       </c>
     </row>
@@ -1851,21 +1857,21 @@
       <c r="J18" s="9">
         <v>0</v>
       </c>
-      <c r="K18" s="39">
-        <v>0</v>
-      </c>
-      <c r="L18" s="39"/>
+      <c r="K18" s="59">
+        <v>0</v>
+      </c>
+      <c r="L18" s="59"/>
       <c r="M18" s="9">
         <v>0</v>
       </c>
       <c r="N18" s="9">
         <v>150</v>
       </c>
-      <c r="O18" s="69">
+      <c r="O18" s="58">
         <v>100</v>
       </c>
-      <c r="P18" s="39"/>
-      <c r="Q18" s="65" t="s">
+      <c r="P18" s="59"/>
+      <c r="Q18" s="55" t="s">
         <v>96</v>
       </c>
     </row>
@@ -1884,31 +1890,31 @@
       <c r="J19" s="9">
         <v>1</v>
       </c>
-      <c r="K19" s="39">
+      <c r="K19" s="59">
         <v>2</v>
       </c>
-      <c r="L19" s="39"/>
+      <c r="L19" s="59"/>
       <c r="M19" s="9">
         <v>2</v>
       </c>
       <c r="N19" s="9">
         <v>651</v>
       </c>
-      <c r="O19" s="69">
+      <c r="O19" s="58">
         <v>85</v>
       </c>
-      <c r="P19" s="39"/>
-      <c r="Q19" s="65" t="s">
+      <c r="P19" s="59"/>
+      <c r="Q19" s="55" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="20" spans="2:17" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="37" t="s">
+      <c r="B20" s="63" t="s">
         <v>39</v>
       </c>
-      <c r="C20" s="37"/>
-      <c r="D20" s="37"/>
-      <c r="E20" s="37"/>
+      <c r="C20" s="63"/>
+      <c r="D20" s="63"/>
+      <c r="E20" s="63"/>
       <c r="G20" s="30" t="s">
         <v>98</v>
       </c>
@@ -1921,21 +1927,21 @@
       <c r="J20" s="31" t="s">
         <v>98</v>
       </c>
-      <c r="K20" s="41" t="s">
+      <c r="K20" s="66" t="s">
         <v>98</v>
       </c>
-      <c r="L20" s="41"/>
+      <c r="L20" s="66"/>
       <c r="M20" s="31" t="s">
         <v>98</v>
       </c>
       <c r="N20" s="31" t="s">
         <v>98</v>
       </c>
-      <c r="O20" s="67" t="s">
+      <c r="O20" s="68" t="s">
         <v>117</v>
       </c>
-      <c r="P20" s="67"/>
-      <c r="Q20" s="66" t="s">
+      <c r="P20" s="68"/>
+      <c r="Q20" s="56" t="s">
         <v>98</v>
       </c>
     </row>
@@ -1968,16 +1974,16 @@
       <c r="E22" s="14">
         <v>150</v>
       </c>
-      <c r="G22" s="37" t="s">
-        <v>118</v>
-      </c>
-      <c r="H22" s="37"/>
-      <c r="I22" s="37"/>
-      <c r="J22" s="37"/>
-      <c r="L22" s="45" t="s">
+      <c r="G22" s="63" t="s">
+        <v>0</v>
+      </c>
+      <c r="H22" s="63"/>
+      <c r="I22" s="63"/>
+      <c r="J22" s="63"/>
+      <c r="L22" s="62" t="s">
         <v>101</v>
       </c>
-      <c r="M22" s="45"/>
+      <c r="M22" s="62"/>
     </row>
     <row r="23" spans="2:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="3">
@@ -1992,10 +1998,10 @@
       <c r="E23" s="14">
         <v>160</v>
       </c>
-      <c r="G23" s="70" t="s">
+      <c r="G23" s="60" t="s">
         <v>99</v>
       </c>
-      <c r="H23" s="42"/>
+      <c r="H23" s="61"/>
       <c r="I23" s="24" t="s">
         <v>1</v>
       </c>
@@ -2024,10 +2030,10 @@
       <c r="E24" s="14">
         <v>170</v>
       </c>
-      <c r="G24" s="38">
+      <c r="G24" s="64">
         <v>1</v>
       </c>
-      <c r="H24" s="39"/>
+      <c r="H24" s="59"/>
       <c r="I24" s="9">
         <v>3</v>
       </c>
@@ -2054,10 +2060,10 @@
       <c r="E25" s="14">
         <v>180</v>
       </c>
-      <c r="G25" s="38">
+      <c r="G25" s="64">
         <v>2</v>
       </c>
-      <c r="H25" s="39"/>
+      <c r="H25" s="59"/>
       <c r="I25" s="9">
         <v>4</v>
       </c>
@@ -2084,10 +2090,10 @@
       <c r="E26" s="14">
         <v>190</v>
       </c>
-      <c r="G26" s="38">
+      <c r="G26" s="64">
         <v>2</v>
       </c>
-      <c r="H26" s="39"/>
+      <c r="H26" s="59"/>
       <c r="I26" s="9">
         <v>5</v>
       </c>
@@ -2114,10 +2120,10 @@
       <c r="E27" s="15">
         <v>200</v>
       </c>
-      <c r="G27" s="38">
+      <c r="G27" s="64">
         <v>2</v>
       </c>
-      <c r="H27" s="39"/>
+      <c r="H27" s="59"/>
       <c r="I27" s="12">
         <v>3</v>
       </c>
@@ -2128,10 +2134,10 @@
     <row r="28" spans="2:17" x14ac:dyDescent="0.25">
       <c r="D28" s="11"/>
       <c r="E28" s="11"/>
-      <c r="G28" s="38">
+      <c r="G28" s="64">
         <v>2</v>
       </c>
-      <c r="H28" s="39"/>
+      <c r="H28" s="59"/>
       <c r="I28" s="12">
         <v>7</v>
       </c>
@@ -2140,16 +2146,16 @@
       </c>
     </row>
     <row r="29" spans="2:17" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B29" s="37" t="s">
+      <c r="B29" s="63" t="s">
         <v>66</v>
       </c>
-      <c r="C29" s="37"/>
-      <c r="D29" s="37"/>
-      <c r="E29" s="37"/>
-      <c r="G29" s="40" t="s">
+      <c r="C29" s="63"/>
+      <c r="D29" s="63"/>
+      <c r="E29" s="63"/>
+      <c r="G29" s="65" t="s">
         <v>98</v>
       </c>
-      <c r="H29" s="41"/>
+      <c r="H29" s="66"/>
       <c r="I29" s="32" t="s">
         <v>98</v>
       </c>
@@ -2184,14 +2190,18 @@
       <c r="E31" s="14">
         <v>0</v>
       </c>
-      <c r="G31" s="37" t="s">
+      <c r="G31" s="63" t="s">
         <v>103</v>
       </c>
-      <c r="H31" s="37"/>
-      <c r="I31" s="37"/>
-      <c r="J31" s="37"/>
-      <c r="K31" s="37"/>
-      <c r="L31" s="37"/>
+      <c r="H31" s="63"/>
+      <c r="I31" s="63"/>
+      <c r="J31" s="63"/>
+      <c r="K31" s="63"/>
+      <c r="L31" s="63"/>
+      <c r="M31" s="63"/>
+      <c r="N31" s="63"/>
+      <c r="O31" s="63"/>
+      <c r="P31" s="63"/>
     </row>
     <row r="32" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B32" s="3">
@@ -2209,17 +2219,27 @@
       <c r="G32" s="23" t="s">
         <v>115</v>
       </c>
-      <c r="H32" s="42" t="s">
+      <c r="H32" s="61" t="s">
         <v>92</v>
       </c>
-      <c r="I32" s="42"/>
-      <c r="J32" s="42" t="s">
+      <c r="I32" s="61"/>
+      <c r="J32" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="K32" s="42"/>
-      <c r="L32" s="43"/>
-    </row>
-    <row r="33" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="K32" s="61"/>
+      <c r="L32" s="61"/>
+      <c r="M32" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="N32" s="61" t="s">
+        <v>119</v>
+      </c>
+      <c r="O32" s="61"/>
+      <c r="P32" s="25" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="33" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B33" s="3">
         <v>2</v>
       </c>
@@ -2235,17 +2255,27 @@
       <c r="G33" s="21">
         <v>0</v>
       </c>
-      <c r="H33" s="39" t="s">
+      <c r="H33" s="59" t="s">
         <v>104</v>
       </c>
-      <c r="I33" s="39"/>
-      <c r="J33" s="39" t="s">
+      <c r="I33" s="59"/>
+      <c r="J33" s="59" t="s">
         <v>34</v>
       </c>
-      <c r="K33" s="39"/>
-      <c r="L33" s="44"/>
-    </row>
-    <row r="34" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="K33" s="59"/>
+      <c r="L33" s="59"/>
+      <c r="M33" s="1">
+        <v>26</v>
+      </c>
+      <c r="N33" s="69">
+        <v>3</v>
+      </c>
+      <c r="O33" s="69"/>
+      <c r="P33" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B34" s="3">
         <v>3</v>
       </c>
@@ -2261,17 +2291,27 @@
       <c r="G34" s="21">
         <v>1</v>
       </c>
-      <c r="H34" s="39" t="s">
+      <c r="H34" s="59" t="s">
         <v>105</v>
       </c>
-      <c r="I34" s="39"/>
-      <c r="J34" s="39" t="s">
+      <c r="I34" s="59"/>
+      <c r="J34" s="59" t="s">
         <v>36</v>
       </c>
-      <c r="K34" s="39"/>
-      <c r="L34" s="44"/>
-    </row>
-    <row r="35" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="K34" s="59"/>
+      <c r="L34" s="59"/>
+      <c r="M34" s="1">
+        <v>3</v>
+      </c>
+      <c r="N34" s="69">
+        <v>3</v>
+      </c>
+      <c r="O34" s="69"/>
+      <c r="P34" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B35" s="3">
         <v>4</v>
       </c>
@@ -2287,17 +2327,27 @@
       <c r="G35" s="21">
         <v>2</v>
       </c>
-      <c r="H35" s="39" t="s">
+      <c r="H35" s="59" t="s">
         <v>106</v>
       </c>
-      <c r="I35" s="39"/>
-      <c r="J35" s="39" t="s">
+      <c r="I35" s="59"/>
+      <c r="J35" s="59" t="s">
         <v>35</v>
       </c>
-      <c r="K35" s="39"/>
-      <c r="L35" s="44"/>
-    </row>
-    <row r="36" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K35" s="59"/>
+      <c r="L35" s="59"/>
+      <c r="M35" s="1">
+        <v>10</v>
+      </c>
+      <c r="N35" s="69">
+        <v>3</v>
+      </c>
+      <c r="O35" s="69"/>
+      <c r="P35" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B36" s="6">
         <v>5</v>
       </c>
@@ -2313,35 +2363,45 @@
       <c r="G36" s="21">
         <v>3</v>
       </c>
-      <c r="H36" s="39" t="s">
+      <c r="H36" s="59" t="s">
         <v>107</v>
       </c>
-      <c r="I36" s="39"/>
-      <c r="J36" s="39" t="s">
+      <c r="I36" s="59"/>
+      <c r="J36" s="59" t="s">
         <v>108</v>
       </c>
-      <c r="K36" s="39"/>
-      <c r="L36" s="44"/>
-    </row>
-    <row r="37" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="K36" s="59"/>
+      <c r="L36" s="59"/>
+      <c r="M36" s="7">
+        <v>18</v>
+      </c>
+      <c r="N36" s="70">
+        <v>3</v>
+      </c>
+      <c r="O36" s="70"/>
+      <c r="P36" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="2:16" x14ac:dyDescent="0.25">
       <c r="D37" s="11"/>
       <c r="E37" s="11"/>
-      <c r="G37" s="46"/>
-      <c r="H37" s="46"/>
-      <c r="I37" s="46"/>
-      <c r="J37" s="46"/>
-      <c r="K37" s="46"/>
-      <c r="L37" s="46"/>
-    </row>
-    <row r="38" spans="2:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B38" s="37" t="s">
+      <c r="G37" s="37"/>
+      <c r="H37" s="37"/>
+      <c r="I37" s="37"/>
+      <c r="J37" s="37"/>
+      <c r="K37" s="37"/>
+      <c r="L37" s="37"/>
+    </row>
+    <row r="38" spans="2:16" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B38" s="63" t="s">
         <v>74</v>
       </c>
-      <c r="C38" s="37"/>
-      <c r="D38" s="37"/>
-      <c r="E38" s="37"/>
-    </row>
-    <row r="39" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C38" s="63"/>
+      <c r="D38" s="63"/>
+      <c r="E38" s="63"/>
+    </row>
+    <row r="39" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B39" s="23" t="s">
         <v>50</v>
       </c>
@@ -2355,7 +2415,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="40" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B40" s="3">
         <v>0</v>
       </c>
@@ -2369,7 +2429,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="41" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B41" s="3">
         <v>1</v>
       </c>
@@ -2383,7 +2443,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="42" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B42" s="3">
         <v>2</v>
       </c>
@@ -2397,7 +2457,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="43" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B43" s="3">
         <v>3</v>
       </c>
@@ -2411,7 +2471,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="44" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B44" s="3">
         <v>4</v>
       </c>
@@ -2425,7 +2485,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="45" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B45" s="6">
         <v>5</v>
       </c>
@@ -2440,22 +2500,17 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="36">
-    <mergeCell ref="R2:V2"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="J36:L36"/>
-    <mergeCell ref="J35:L35"/>
-    <mergeCell ref="J34:L34"/>
-    <mergeCell ref="J33:L33"/>
-    <mergeCell ref="H36:I36"/>
-    <mergeCell ref="H35:I35"/>
-    <mergeCell ref="H34:I34"/>
-    <mergeCell ref="H33:I33"/>
-    <mergeCell ref="H32:I32"/>
-    <mergeCell ref="L22:M22"/>
-    <mergeCell ref="J32:L32"/>
-    <mergeCell ref="G31:L31"/>
+  <mergeCells count="41">
+    <mergeCell ref="N33:O33"/>
+    <mergeCell ref="N34:O34"/>
+    <mergeCell ref="N35:O35"/>
+    <mergeCell ref="N36:O36"/>
+    <mergeCell ref="G31:P31"/>
+    <mergeCell ref="G22:J22"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B20:E20"/>
+    <mergeCell ref="N32:O32"/>
     <mergeCell ref="B29:E29"/>
     <mergeCell ref="B38:E38"/>
     <mergeCell ref="G16:P16"/>
@@ -2472,11 +2527,21 @@
     <mergeCell ref="O17:P17"/>
     <mergeCell ref="O20:P20"/>
     <mergeCell ref="O19:P19"/>
+    <mergeCell ref="R2:V2"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="J36:L36"/>
+    <mergeCell ref="J35:L35"/>
+    <mergeCell ref="J34:L34"/>
+    <mergeCell ref="J33:L33"/>
+    <mergeCell ref="H36:I36"/>
+    <mergeCell ref="H35:I35"/>
+    <mergeCell ref="H34:I34"/>
+    <mergeCell ref="H33:I33"/>
+    <mergeCell ref="H32:I32"/>
+    <mergeCell ref="L22:M22"/>
+    <mergeCell ref="J32:L32"/>
     <mergeCell ref="G2:M2"/>
-    <mergeCell ref="G22:J22"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B20:E20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>